<commit_message>
Code pushed of verifying company in side bar and companies drop down.
</commit_message>
<xml_diff>
--- a/Keytrack_Framework/TestData/Data.xlsx
+++ b/Keytrack_Framework/TestData/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16305" windowHeight="6060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16710" windowHeight="4065"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <t>Abc12345</t>
   </si>
   <si>
-    <t>tahirgeeks+44@gmail.com</t>
+    <t>tahirgeeks+45@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>